<commit_message>
Update Prasanna Skills Audit.xlsx
</commit_message>
<xml_diff>
--- a/Skill Audit/Prasanna Skills Audit.xlsx
+++ b/Skill Audit/Prasanna Skills Audit.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakri\Documents\GitHub\Group3\Skill Audit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6C3E99-1291-4585-9941-DF6CE3B8449E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>NO#</t>
   </si>
@@ -51,9 +57,6 @@
     <t>Skill Level: 1 (No Knowledge) - 5 (Competent)</t>
   </si>
   <si>
-    <t xml:space="preserve">Date Reviewed: </t>
-  </si>
-  <si>
     <t>Java Script</t>
   </si>
   <si>
@@ -169,12 +172,45 @@
   </si>
   <si>
     <t>To make online payment through paypal</t>
+  </si>
+  <si>
+    <t>apex oracle</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>Trello</t>
+  </si>
+  <si>
+    <t>One drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apex Oracle Online </t>
+  </si>
+  <si>
+    <t>To manage and store data in a user friendly basis.</t>
+  </si>
+  <si>
+    <t>Slack Application</t>
+  </si>
+  <si>
+    <t>For the communication of the team members</t>
+  </si>
+  <si>
+    <t>To make sure that the task is done in a proper organized way</t>
+  </si>
+  <si>
+    <t>For the knowledge of files and folders storation</t>
+  </si>
+  <si>
+    <t>Date Reviewed: 02/27/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -233,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -371,12 +407,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -392,9 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -439,8 +500,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -781,89 +857,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="32.125" customWidth="1"/>
-    <col min="5" max="5" width="32.375" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="7" max="7" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.875" customWidth="1"/>
+    <col min="4" max="4" width="32.09765625" customWidth="1"/>
+    <col min="5" max="5" width="32.3984375" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" customWidth="1"/>
+    <col min="7" max="7" width="27.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="9"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -882,340 +958,404 @@
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="23" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="F7" s="5">
         <v>15</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="8">
         <v>43894</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="5">
         <v>15</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="8">
         <v>43955</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="F9" s="5">
         <v>10</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="8">
         <v>44016</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F10" s="5">
         <v>5</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="8">
         <v>43834</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="F11" s="5">
         <v>10</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>31</v>
+      <c r="G11" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5">
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F12" s="5">
         <v>5</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>31</v>
+      <c r="G12" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="F13" s="5">
         <v>10</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>30</v>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="24">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="24">
+        <v>4</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5">
+      <c r="E14" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="24">
+        <v>10</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="26">
+        <v>9</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="26">
         <v>4</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="D15" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="26">
+        <v>10</v>
+      </c>
+      <c r="G15" s="27">
+        <v>43835</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26">
+        <v>10</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="26">
+        <v>3</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="26">
+        <v>8</v>
+      </c>
+      <c r="G16" s="27">
+        <v>43835</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="26">
+        <v>11</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="26">
+        <v>3</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="26">
+        <v>12</v>
+      </c>
+      <c r="G17" s="27">
+        <v>43835</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="26">
+        <v>12</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="26">
+        <v>2</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="26">
+        <v>8</v>
+      </c>
+      <c r="G18" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5">
-        <v>10</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>9</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="H18" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="26">
+        <v>13</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="26">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="5">
-        <v>10</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="D19" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="26">
+        <v>5</v>
+      </c>
+      <c r="G19" s="27">
         <v>43835</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>10</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="H19" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="26">
+        <v>14</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="26">
         <v>3</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="5">
-        <v>8</v>
-      </c>
-      <c r="G16" s="7">
+      <c r="D20" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="26">
+        <v>5</v>
+      </c>
+      <c r="G20" s="27">
         <v>43835</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="H20" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="26">
+        <v>15</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="26">
         <v>3</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="1">
-        <v>12</v>
-      </c>
-      <c r="G17" s="24">
+      <c r="D21" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="26">
+        <v>4</v>
+      </c>
+      <c r="G21" s="27">
         <v>43835</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1225,7 +1365,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1235,7 +1375,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1245,7 +1385,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1255,7 +1395,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>

</xml_diff>